<commit_message>
updating gui, advance tree logic
</commit_message>
<xml_diff>
--- a/refined_divisions/test_10.xlsx
+++ b/refined_divisions/test_10.xlsx
@@ -190,7 +190,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -203,9 +205,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -226,6 +226,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -277,44 +313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -322,11 +322,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -334,7 +334,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -709,8 +709,8 @@
   </sheetPr>
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -721,22 +721,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="8.1" customHeight="1" s="12">
-      <c r="B1" s="31" t="inlineStr">
+      <c r="B1" s="40" t="inlineStr">
         <is>
           <t>Round of 16</t>
         </is>
       </c>
-      <c r="E1" s="31" t="inlineStr">
+      <c r="E1" s="40" t="inlineStr">
         <is>
           <t>Quarter-Final</t>
         </is>
       </c>
-      <c r="H1" s="31" t="inlineStr">
+      <c r="H1" s="40" t="inlineStr">
         <is>
           <t>Semi-Final</t>
         </is>
       </c>
-      <c r="K1" s="31" t="inlineStr">
+      <c r="K1" s="40" t="inlineStr">
         <is>
           <t>Final</t>
         </is>
@@ -769,15 +769,15 @@
       <c r="C4" s="46" t="n"/>
     </row>
     <row r="5" ht="8.1" customHeight="1" s="12">
-      <c r="B5" s="41" t="n"/>
-      <c r="C5" s="41" t="n"/>
+      <c r="B5" s="14" t="n"/>
+      <c r="C5" s="14" t="n"/>
       <c r="D5" s="9" t="n"/>
       <c r="E5" s="43" t="inlineStr"/>
       <c r="F5" s="44" t="n"/>
     </row>
     <row r="6" ht="8.1" customHeight="1" s="12">
-      <c r="B6" s="41" t="n"/>
-      <c r="C6" s="41" t="n"/>
+      <c r="B6" s="14" t="n"/>
+      <c r="C6" s="14" t="n"/>
       <c r="D6" s="3" t="n"/>
       <c r="E6" s="45" t="inlineStr"/>
       <c r="F6" s="46" t="n"/>
@@ -800,8 +800,8 @@
         </is>
       </c>
       <c r="C7" s="44" t="n"/>
-      <c r="E7" s="41" t="n"/>
-      <c r="F7" s="41" t="n"/>
+      <c r="E7" s="14" t="n"/>
+      <c r="F7" s="14" t="n"/>
       <c r="G7" s="8" t="n"/>
       <c r="K7" s="8" t="n"/>
       <c r="Q7" s="50" t="n"/>
@@ -813,17 +813,17 @@
         </is>
       </c>
       <c r="C8" s="46" t="n"/>
-      <c r="E8" s="41" t="n"/>
-      <c r="F8" s="41" t="n"/>
+      <c r="E8" s="14" t="n"/>
+      <c r="F8" s="14" t="n"/>
       <c r="G8" s="8" t="n"/>
       <c r="K8" s="8" t="n"/>
       <c r="Q8" s="50" t="n"/>
     </row>
     <row r="9" ht="8.1" customHeight="1" s="12">
-      <c r="B9" s="41" t="n"/>
-      <c r="C9" s="41" t="n"/>
-      <c r="E9" s="41" t="n"/>
-      <c r="F9" s="41" t="n"/>
+      <c r="B9" s="14" t="n"/>
+      <c r="C9" s="14" t="n"/>
+      <c r="E9" s="14" t="n"/>
+      <c r="F9" s="14" t="n"/>
       <c r="G9" s="9" t="n"/>
       <c r="H9" s="43" t="n"/>
       <c r="I9" s="44" t="n"/>
@@ -836,10 +836,10 @@
       <c r="Q9" s="46" t="n"/>
     </row>
     <row r="10" ht="8.1" customHeight="1" s="12">
-      <c r="B10" s="41" t="n"/>
-      <c r="C10" s="41" t="n"/>
-      <c r="E10" s="41" t="n"/>
-      <c r="F10" s="41" t="n"/>
+      <c r="B10" s="14" t="n"/>
+      <c r="C10" s="14" t="n"/>
+      <c r="E10" s="14" t="n"/>
+      <c r="F10" s="14" t="n"/>
       <c r="G10" s="8" t="n"/>
       <c r="H10" s="45" t="n"/>
       <c r="I10" s="46" t="n"/>
@@ -851,26 +851,26 @@
         </is>
       </c>
       <c r="C11" s="44" t="n"/>
-      <c r="E11" s="41" t="n"/>
-      <c r="F11" s="41" t="n"/>
+      <c r="E11" s="14" t="n"/>
+      <c r="F11" s="14" t="n"/>
       <c r="G11" s="8" t="n"/>
-      <c r="H11" s="41" t="n"/>
-      <c r="I11" s="41" t="n"/>
+      <c r="H11" s="14" t="n"/>
+      <c r="I11" s="14" t="n"/>
       <c r="J11" s="8" t="n"/>
     </row>
     <row r="12" ht="8.1" customHeight="1" s="12">
       <c r="B12" s="45" t="inlineStr"/>
       <c r="C12" s="46" t="n"/>
-      <c r="E12" s="41" t="n"/>
-      <c r="F12" s="41" t="n"/>
+      <c r="E12" s="14" t="n"/>
+      <c r="F12" s="14" t="n"/>
       <c r="G12" s="8" t="n"/>
-      <c r="H12" s="41" t="n"/>
-      <c r="I12" s="41" t="n"/>
+      <c r="H12" s="14" t="n"/>
+      <c r="I12" s="14" t="n"/>
       <c r="J12" s="8" t="n"/>
     </row>
     <row r="13" ht="8.1" customHeight="1" s="12">
-      <c r="B13" s="41" t="n"/>
-      <c r="C13" s="41" t="n"/>
+      <c r="B13" s="14" t="n"/>
+      <c r="C13" s="14" t="n"/>
       <c r="D13" s="9" t="n"/>
       <c r="E13" s="49" t="inlineStr">
         <is>
@@ -878,13 +878,13 @@
         </is>
       </c>
       <c r="F13" s="44" t="n"/>
-      <c r="H13" s="41" t="n"/>
-      <c r="I13" s="41" t="n"/>
+      <c r="H13" s="14" t="n"/>
+      <c r="I13" s="14" t="n"/>
       <c r="J13" s="8" t="n"/>
     </row>
     <row r="14" ht="8.1" customHeight="1" s="12">
-      <c r="B14" s="41" t="n"/>
-      <c r="C14" s="41" t="n"/>
+      <c r="B14" s="14" t="n"/>
+      <c r="C14" s="14" t="n"/>
       <c r="D14" s="3" t="n"/>
       <c r="E14" s="51" t="inlineStr">
         <is>
@@ -892,8 +892,8 @@
         </is>
       </c>
       <c r="F14" s="46" t="n"/>
-      <c r="H14" s="41" t="n"/>
-      <c r="I14" s="41" t="n"/>
+      <c r="H14" s="14" t="n"/>
+      <c r="I14" s="14" t="n"/>
       <c r="J14" s="8" t="n"/>
     </row>
     <row r="15" ht="8.1" customHeight="1" s="12">
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="C15" s="44" t="n"/>
-      <c r="E15" s="41" t="n"/>
-      <c r="F15" s="41" t="n"/>
-      <c r="H15" s="41" t="n"/>
-      <c r="I15" s="41" t="n"/>
+      <c r="E15" s="14" t="n"/>
+      <c r="F15" s="14" t="n"/>
+      <c r="H15" s="14" t="n"/>
+      <c r="I15" s="14" t="n"/>
       <c r="J15" s="8" t="n"/>
     </row>
     <row r="16" ht="8.1" customHeight="1" s="12">
@@ -916,30 +916,30 @@
         </is>
       </c>
       <c r="C16" s="46" t="n"/>
-      <c r="E16" s="41" t="n"/>
-      <c r="F16" s="41" t="n"/>
-      <c r="H16" s="41" t="n"/>
-      <c r="I16" s="41" t="n"/>
+      <c r="E16" s="14" t="n"/>
+      <c r="F16" s="14" t="n"/>
+      <c r="H16" s="14" t="n"/>
+      <c r="I16" s="14" t="n"/>
       <c r="J16" s="8" t="n"/>
     </row>
     <row r="17" ht="8.1" customHeight="1" s="12">
-      <c r="B17" s="41" t="n"/>
-      <c r="C17" s="41" t="n"/>
-      <c r="E17" s="41" t="n"/>
-      <c r="F17" s="41" t="n"/>
-      <c r="H17" s="41" t="n"/>
-      <c r="I17" s="41" t="n"/>
+      <c r="B17" s="14" t="n"/>
+      <c r="C17" s="14" t="n"/>
+      <c r="E17" s="14" t="n"/>
+      <c r="F17" s="14" t="n"/>
+      <c r="H17" s="14" t="n"/>
+      <c r="I17" s="14" t="n"/>
       <c r="J17" s="9" t="n"/>
       <c r="K17" s="43" t="n"/>
       <c r="L17" s="44" t="n"/>
     </row>
     <row r="18" ht="8.1" customHeight="1" s="12">
-      <c r="B18" s="41" t="n"/>
-      <c r="C18" s="41" t="n"/>
-      <c r="E18" s="41" t="n"/>
-      <c r="F18" s="41" t="n"/>
-      <c r="H18" s="41" t="n"/>
-      <c r="I18" s="41" t="n"/>
+      <c r="B18" s="14" t="n"/>
+      <c r="C18" s="14" t="n"/>
+      <c r="E18" s="14" t="n"/>
+      <c r="F18" s="14" t="n"/>
+      <c r="H18" s="14" t="n"/>
+      <c r="I18" s="14" t="n"/>
       <c r="J18" s="8" t="n"/>
       <c r="K18" s="45" t="n"/>
       <c r="L18" s="46" t="n"/>
@@ -951,13 +951,13 @@
         </is>
       </c>
       <c r="C19" s="44" t="n"/>
-      <c r="E19" s="41" t="n"/>
-      <c r="F19" s="41" t="n"/>
-      <c r="H19" s="41" t="n"/>
-      <c r="I19" s="41" t="n"/>
+      <c r="E19" s="14" t="n"/>
+      <c r="F19" s="14" t="n"/>
+      <c r="H19" s="14" t="n"/>
+      <c r="I19" s="14" t="n"/>
       <c r="J19" s="8" t="n"/>
-      <c r="K19" s="41" t="n"/>
-      <c r="L19" s="41" t="n"/>
+      <c r="K19" s="14" t="n"/>
+      <c r="L19" s="14" t="n"/>
       <c r="M19" s="8" t="n"/>
     </row>
     <row r="20" ht="8.1" customHeight="1" s="12">
@@ -967,18 +967,18 @@
         </is>
       </c>
       <c r="C20" s="46" t="n"/>
-      <c r="E20" s="41" t="n"/>
-      <c r="F20" s="41" t="n"/>
-      <c r="H20" s="41" t="n"/>
-      <c r="I20" s="41" t="n"/>
+      <c r="E20" s="14" t="n"/>
+      <c r="F20" s="14" t="n"/>
+      <c r="H20" s="14" t="n"/>
+      <c r="I20" s="14" t="n"/>
       <c r="J20" s="8" t="n"/>
-      <c r="K20" s="41" t="n"/>
-      <c r="L20" s="41" t="n"/>
+      <c r="K20" s="14" t="n"/>
+      <c r="L20" s="14" t="n"/>
       <c r="M20" s="8" t="n"/>
     </row>
     <row r="21" ht="8.1" customHeight="1" s="12">
-      <c r="B21" s="41" t="n"/>
-      <c r="C21" s="41" t="n"/>
+      <c r="B21" s="14" t="n"/>
+      <c r="C21" s="14" t="n"/>
       <c r="D21" s="9" t="n"/>
       <c r="E21" s="43" t="inlineStr">
         <is>
@@ -986,16 +986,16 @@
         </is>
       </c>
       <c r="F21" s="44" t="n"/>
-      <c r="H21" s="41" t="n"/>
-      <c r="I21" s="41" t="n"/>
+      <c r="H21" s="14" t="n"/>
+      <c r="I21" s="14" t="n"/>
       <c r="J21" s="8" t="n"/>
-      <c r="K21" s="41" t="n"/>
-      <c r="L21" s="41" t="n"/>
+      <c r="K21" s="14" t="n"/>
+      <c r="L21" s="14" t="n"/>
       <c r="M21" s="8" t="n"/>
     </row>
     <row r="22" ht="8.1" customHeight="1" s="12">
-      <c r="B22" s="41" t="n"/>
-      <c r="C22" s="41" t="n"/>
+      <c r="B22" s="14" t="n"/>
+      <c r="C22" s="14" t="n"/>
       <c r="D22" s="3" t="n"/>
       <c r="E22" s="45" t="inlineStr">
         <is>
@@ -1003,11 +1003,11 @@
         </is>
       </c>
       <c r="F22" s="46" t="n"/>
-      <c r="H22" s="41" t="n"/>
-      <c r="I22" s="41" t="n"/>
+      <c r="H22" s="14" t="n"/>
+      <c r="I22" s="14" t="n"/>
       <c r="J22" s="8" t="n"/>
-      <c r="K22" s="41" t="n"/>
-      <c r="L22" s="41" t="n"/>
+      <c r="K22" s="14" t="n"/>
+      <c r="L22" s="14" t="n"/>
       <c r="M22" s="8" t="n"/>
     </row>
     <row r="23" ht="8.1" customHeight="1" s="12">
@@ -1017,51 +1017,51 @@
         </is>
       </c>
       <c r="C23" s="44" t="n"/>
-      <c r="E23" s="41" t="n"/>
-      <c r="F23" s="41" t="n"/>
+      <c r="E23" s="14" t="n"/>
+      <c r="F23" s="14" t="n"/>
       <c r="G23" s="8" t="n"/>
-      <c r="H23" s="41" t="n"/>
-      <c r="I23" s="41" t="n"/>
+      <c r="H23" s="14" t="n"/>
+      <c r="I23" s="14" t="n"/>
       <c r="J23" s="8" t="n"/>
-      <c r="K23" s="41" t="n"/>
-      <c r="L23" s="41" t="n"/>
+      <c r="K23" s="14" t="n"/>
+      <c r="L23" s="14" t="n"/>
       <c r="M23" s="8" t="n"/>
     </row>
     <row r="24" ht="8.1" customHeight="1" s="12">
       <c r="B24" s="51" t="inlineStr"/>
       <c r="C24" s="46" t="n"/>
-      <c r="E24" s="41" t="n"/>
-      <c r="F24" s="41" t="n"/>
+      <c r="E24" s="14" t="n"/>
+      <c r="F24" s="14" t="n"/>
       <c r="G24" s="8" t="n"/>
-      <c r="H24" s="41" t="n"/>
-      <c r="I24" s="41" t="n"/>
+      <c r="H24" s="14" t="n"/>
+      <c r="I24" s="14" t="n"/>
       <c r="J24" s="8" t="n"/>
-      <c r="K24" s="41" t="n"/>
-      <c r="L24" s="41" t="n"/>
+      <c r="K24" s="14" t="n"/>
+      <c r="L24" s="14" t="n"/>
       <c r="M24" s="8" t="n"/>
     </row>
     <row r="25" ht="8.1" customHeight="1" s="12">
-      <c r="B25" s="41" t="n"/>
-      <c r="C25" s="41" t="n"/>
-      <c r="E25" s="41" t="n"/>
-      <c r="F25" s="41" t="n"/>
+      <c r="B25" s="14" t="n"/>
+      <c r="C25" s="14" t="n"/>
+      <c r="E25" s="14" t="n"/>
+      <c r="F25" s="14" t="n"/>
       <c r="G25" s="9" t="n"/>
       <c r="H25" s="49" t="n"/>
       <c r="I25" s="44" t="n"/>
-      <c r="K25" s="41" t="n"/>
-      <c r="L25" s="41" t="n"/>
+      <c r="K25" s="14" t="n"/>
+      <c r="L25" s="14" t="n"/>
       <c r="M25" s="8" t="n"/>
     </row>
     <row r="26" ht="8.1" customHeight="1" s="12">
-      <c r="B26" s="41" t="n"/>
-      <c r="C26" s="41" t="n"/>
-      <c r="E26" s="41" t="n"/>
-      <c r="F26" s="41" t="n"/>
+      <c r="B26" s="14" t="n"/>
+      <c r="C26" s="14" t="n"/>
+      <c r="E26" s="14" t="n"/>
+      <c r="F26" s="14" t="n"/>
       <c r="G26" s="8" t="n"/>
       <c r="H26" s="51" t="n"/>
       <c r="I26" s="46" t="n"/>
-      <c r="K26" s="41" t="n"/>
-      <c r="L26" s="41" t="n"/>
+      <c r="K26" s="14" t="n"/>
+      <c r="L26" s="14" t="n"/>
       <c r="M26" s="8" t="n"/>
     </row>
     <row r="27" ht="8.1" customHeight="1" s="12">
@@ -1071,30 +1071,30 @@
         </is>
       </c>
       <c r="C27" s="44" t="n"/>
-      <c r="E27" s="41" t="n"/>
-      <c r="F27" s="41" t="n"/>
+      <c r="E27" s="14" t="n"/>
+      <c r="F27" s="14" t="n"/>
       <c r="G27" s="8" t="n"/>
-      <c r="H27" s="41" t="n"/>
-      <c r="I27" s="41" t="n"/>
-      <c r="K27" s="41" t="n"/>
-      <c r="L27" s="41" t="n"/>
+      <c r="H27" s="14" t="n"/>
+      <c r="I27" s="14" t="n"/>
+      <c r="K27" s="14" t="n"/>
+      <c r="L27" s="14" t="n"/>
       <c r="M27" s="8" t="n"/>
     </row>
     <row r="28" ht="8.1" customHeight="1" s="12">
       <c r="B28" s="45" t="inlineStr"/>
       <c r="C28" s="46" t="n"/>
-      <c r="E28" s="41" t="n"/>
-      <c r="F28" s="41" t="n"/>
+      <c r="E28" s="14" t="n"/>
+      <c r="F28" s="14" t="n"/>
       <c r="G28" s="8" t="n"/>
-      <c r="H28" s="41" t="n"/>
-      <c r="I28" s="41" t="n"/>
-      <c r="K28" s="41" t="n"/>
-      <c r="L28" s="41" t="n"/>
+      <c r="H28" s="14" t="n"/>
+      <c r="I28" s="14" t="n"/>
+      <c r="K28" s="14" t="n"/>
+      <c r="L28" s="14" t="n"/>
       <c r="M28" s="8" t="n"/>
     </row>
     <row r="29" ht="8.1" customHeight="1" s="12">
-      <c r="B29" s="41" t="n"/>
-      <c r="C29" s="41" t="n"/>
+      <c r="B29" s="14" t="n"/>
+      <c r="C29" s="14" t="n"/>
       <c r="D29" s="9" t="n"/>
       <c r="E29" s="49" t="inlineStr">
         <is>
@@ -1102,15 +1102,15 @@
         </is>
       </c>
       <c r="F29" s="44" t="n"/>
-      <c r="H29" s="41" t="n"/>
-      <c r="I29" s="41" t="n"/>
-      <c r="K29" s="41" t="n"/>
-      <c r="L29" s="41" t="n"/>
+      <c r="H29" s="14" t="n"/>
+      <c r="I29" s="14" t="n"/>
+      <c r="K29" s="14" t="n"/>
+      <c r="L29" s="14" t="n"/>
       <c r="M29" s="8" t="n"/>
     </row>
     <row r="30" ht="8.1" customHeight="1" s="12">
-      <c r="B30" s="41" t="n"/>
-      <c r="C30" s="41" t="n"/>
+      <c r="B30" s="14" t="n"/>
+      <c r="C30" s="14" t="n"/>
       <c r="D30" s="3" t="n"/>
       <c r="E30" s="51" t="inlineStr">
         <is>
@@ -1118,10 +1118,10 @@
         </is>
       </c>
       <c r="F30" s="46" t="n"/>
-      <c r="H30" s="41" t="n"/>
-      <c r="I30" s="41" t="n"/>
-      <c r="K30" s="41" t="n"/>
-      <c r="L30" s="41" t="n"/>
+      <c r="H30" s="14" t="n"/>
+      <c r="I30" s="14" t="n"/>
+      <c r="K30" s="14" t="n"/>
+      <c r="L30" s="14" t="n"/>
       <c r="M30" s="8" t="n"/>
     </row>
     <row r="31" ht="8.1" customHeight="1" s="12">
@@ -1131,14 +1131,14 @@
         </is>
       </c>
       <c r="C31" s="44" t="n"/>
-      <c r="E31" s="41" t="n"/>
-      <c r="F31" s="41" t="n"/>
-      <c r="H31" s="41" t="n"/>
-      <c r="I31" s="41" t="n"/>
-      <c r="K31" s="41" t="n"/>
-      <c r="L31" s="41" t="n"/>
+      <c r="E31" s="14" t="n"/>
+      <c r="F31" s="14" t="n"/>
+      <c r="H31" s="14" t="n"/>
+      <c r="I31" s="14" t="n"/>
+      <c r="K31" s="14" t="n"/>
+      <c r="L31" s="14" t="n"/>
       <c r="M31" s="8" t="n"/>
-      <c r="N31" s="31" t="inlineStr">
+      <c r="N31" s="40" t="inlineStr">
         <is>
           <t>Winner</t>
         </is>
@@ -1151,38 +1151,38 @@
         </is>
       </c>
       <c r="C32" s="46" t="n"/>
-      <c r="E32" s="41" t="n"/>
-      <c r="F32" s="41" t="n"/>
-      <c r="H32" s="41" t="n"/>
-      <c r="I32" s="41" t="n"/>
-      <c r="K32" s="41" t="n"/>
-      <c r="L32" s="41" t="n"/>
+      <c r="E32" s="14" t="n"/>
+      <c r="F32" s="14" t="n"/>
+      <c r="H32" s="14" t="n"/>
+      <c r="I32" s="14" t="n"/>
+      <c r="K32" s="14" t="n"/>
+      <c r="L32" s="14" t="n"/>
       <c r="M32" s="8" t="n"/>
       <c r="N32" s="42" t="n"/>
       <c r="O32" s="42" t="n"/>
     </row>
     <row r="33" ht="8.1" customHeight="1" s="12">
-      <c r="B33" s="41" t="n"/>
-      <c r="C33" s="41" t="n"/>
-      <c r="E33" s="41" t="n"/>
-      <c r="F33" s="41" t="n"/>
-      <c r="H33" s="41" t="n"/>
-      <c r="I33" s="41" t="n"/>
-      <c r="K33" s="41" t="n"/>
-      <c r="L33" s="41" t="n"/>
+      <c r="B33" s="14" t="n"/>
+      <c r="C33" s="14" t="n"/>
+      <c r="E33" s="14" t="n"/>
+      <c r="F33" s="14" t="n"/>
+      <c r="H33" s="14" t="n"/>
+      <c r="I33" s="14" t="n"/>
+      <c r="K33" s="14" t="n"/>
+      <c r="L33" s="14" t="n"/>
       <c r="M33" s="9" t="n"/>
       <c r="N33" s="53" t="n"/>
       <c r="O33" s="44" t="n"/>
     </row>
     <row r="34" ht="8.1" customHeight="1" s="12">
-      <c r="B34" s="41" t="n"/>
-      <c r="C34" s="41" t="n"/>
-      <c r="E34" s="41" t="n"/>
-      <c r="F34" s="41" t="n"/>
-      <c r="H34" s="41" t="n"/>
-      <c r="I34" s="41" t="n"/>
-      <c r="K34" s="41" t="n"/>
-      <c r="L34" s="41" t="n"/>
+      <c r="B34" s="14" t="n"/>
+      <c r="C34" s="14" t="n"/>
+      <c r="E34" s="14" t="n"/>
+      <c r="F34" s="14" t="n"/>
+      <c r="H34" s="14" t="n"/>
+      <c r="I34" s="14" t="n"/>
+      <c r="K34" s="14" t="n"/>
+      <c r="L34" s="14" t="n"/>
       <c r="M34" s="8" t="n"/>
       <c r="N34" s="54" t="n"/>
       <c r="O34" s="46" t="n"/>
@@ -1194,12 +1194,12 @@
         </is>
       </c>
       <c r="C35" s="44" t="n"/>
-      <c r="E35" s="41" t="n"/>
-      <c r="F35" s="41" t="n"/>
-      <c r="H35" s="41" t="n"/>
-      <c r="I35" s="41" t="n"/>
-      <c r="K35" s="41" t="n"/>
-      <c r="L35" s="41" t="n"/>
+      <c r="E35" s="14" t="n"/>
+      <c r="F35" s="14" t="n"/>
+      <c r="H35" s="14" t="n"/>
+      <c r="I35" s="14" t="n"/>
+      <c r="K35" s="14" t="n"/>
+      <c r="L35" s="14" t="n"/>
       <c r="M35" s="8" t="n"/>
     </row>
     <row r="36" ht="8.1" customHeight="1" s="12">
@@ -1209,36 +1209,36 @@
         </is>
       </c>
       <c r="C36" s="46" t="n"/>
-      <c r="E36" s="41" t="n"/>
-      <c r="F36" s="41" t="n"/>
-      <c r="H36" s="41" t="n"/>
-      <c r="I36" s="41" t="n"/>
-      <c r="K36" s="41" t="n"/>
-      <c r="L36" s="41" t="n"/>
+      <c r="E36" s="14" t="n"/>
+      <c r="F36" s="14" t="n"/>
+      <c r="H36" s="14" t="n"/>
+      <c r="I36" s="14" t="n"/>
+      <c r="K36" s="14" t="n"/>
+      <c r="L36" s="14" t="n"/>
       <c r="M36" s="8" t="n"/>
     </row>
     <row r="37" ht="8.1" customHeight="1" s="12">
-      <c r="B37" s="41" t="n"/>
-      <c r="C37" s="41" t="n"/>
+      <c r="B37" s="14" t="n"/>
+      <c r="C37" s="14" t="n"/>
       <c r="D37" s="9" t="n"/>
       <c r="E37" s="43" t="inlineStr"/>
       <c r="F37" s="44" t="n"/>
-      <c r="H37" s="41" t="n"/>
-      <c r="I37" s="41" t="n"/>
-      <c r="K37" s="41" t="n"/>
-      <c r="L37" s="41" t="n"/>
+      <c r="H37" s="14" t="n"/>
+      <c r="I37" s="14" t="n"/>
+      <c r="K37" s="14" t="n"/>
+      <c r="L37" s="14" t="n"/>
       <c r="M37" s="8" t="n"/>
     </row>
     <row r="38" ht="8.1" customHeight="1" s="12">
-      <c r="B38" s="41" t="n"/>
-      <c r="C38" s="41" t="n"/>
+      <c r="B38" s="14" t="n"/>
+      <c r="C38" s="14" t="n"/>
       <c r="D38" s="3" t="n"/>
       <c r="E38" s="45" t="inlineStr"/>
       <c r="F38" s="46" t="n"/>
-      <c r="H38" s="41" t="n"/>
-      <c r="I38" s="41" t="n"/>
-      <c r="K38" s="41" t="n"/>
-      <c r="L38" s="41" t="n"/>
+      <c r="H38" s="14" t="n"/>
+      <c r="I38" s="14" t="n"/>
+      <c r="K38" s="14" t="n"/>
+      <c r="L38" s="14" t="n"/>
       <c r="M38" s="8" t="n"/>
     </row>
     <row r="39" ht="8.1" customHeight="1" s="12">
@@ -1248,13 +1248,13 @@
         </is>
       </c>
       <c r="C39" s="44" t="n"/>
-      <c r="E39" s="41" t="n"/>
-      <c r="F39" s="41" t="n"/>
+      <c r="E39" s="14" t="n"/>
+      <c r="F39" s="14" t="n"/>
       <c r="G39" s="8" t="n"/>
-      <c r="H39" s="41" t="n"/>
-      <c r="I39" s="41" t="n"/>
-      <c r="K39" s="41" t="n"/>
-      <c r="L39" s="41" t="n"/>
+      <c r="H39" s="14" t="n"/>
+      <c r="I39" s="14" t="n"/>
+      <c r="K39" s="14" t="n"/>
+      <c r="L39" s="14" t="n"/>
       <c r="M39" s="8" t="n"/>
     </row>
     <row r="40" ht="8.1" customHeight="1" s="12">
@@ -1264,37 +1264,37 @@
         </is>
       </c>
       <c r="C40" s="46" t="n"/>
-      <c r="E40" s="41" t="n"/>
-      <c r="F40" s="41" t="n"/>
+      <c r="E40" s="14" t="n"/>
+      <c r="F40" s="14" t="n"/>
       <c r="G40" s="8" t="n"/>
-      <c r="H40" s="41" t="n"/>
-      <c r="I40" s="41" t="n"/>
-      <c r="K40" s="41" t="n"/>
-      <c r="L40" s="41" t="n"/>
+      <c r="H40" s="14" t="n"/>
+      <c r="I40" s="14" t="n"/>
+      <c r="K40" s="14" t="n"/>
+      <c r="L40" s="14" t="n"/>
       <c r="M40" s="8" t="n"/>
     </row>
     <row r="41" ht="8.1" customHeight="1" s="12">
-      <c r="B41" s="41" t="n"/>
-      <c r="C41" s="41" t="n"/>
-      <c r="E41" s="41" t="n"/>
-      <c r="F41" s="41" t="n"/>
+      <c r="B41" s="14" t="n"/>
+      <c r="C41" s="14" t="n"/>
+      <c r="E41" s="14" t="n"/>
+      <c r="F41" s="14" t="n"/>
       <c r="G41" s="9" t="n"/>
       <c r="H41" s="43" t="n"/>
       <c r="I41" s="44" t="n"/>
-      <c r="K41" s="41" t="n"/>
-      <c r="L41" s="41" t="n"/>
+      <c r="K41" s="14" t="n"/>
+      <c r="L41" s="14" t="n"/>
       <c r="M41" s="8" t="n"/>
     </row>
     <row r="42" ht="8.1" customHeight="1" s="12">
-      <c r="B42" s="41" t="n"/>
-      <c r="C42" s="41" t="n"/>
-      <c r="E42" s="41" t="n"/>
-      <c r="F42" s="41" t="n"/>
+      <c r="B42" s="14" t="n"/>
+      <c r="C42" s="14" t="n"/>
+      <c r="E42" s="14" t="n"/>
+      <c r="F42" s="14" t="n"/>
       <c r="G42" s="8" t="n"/>
       <c r="H42" s="45" t="n"/>
       <c r="I42" s="46" t="n"/>
-      <c r="K42" s="41" t="n"/>
-      <c r="L42" s="41" t="n"/>
+      <c r="K42" s="14" t="n"/>
+      <c r="L42" s="14" t="n"/>
       <c r="M42" s="8" t="n"/>
     </row>
     <row r="43" ht="8.1" customHeight="1" s="12">
@@ -1304,32 +1304,32 @@
         </is>
       </c>
       <c r="C43" s="44" t="n"/>
-      <c r="E43" s="41" t="n"/>
-      <c r="F43" s="41" t="n"/>
+      <c r="E43" s="14" t="n"/>
+      <c r="F43" s="14" t="n"/>
       <c r="G43" s="8" t="n"/>
-      <c r="H43" s="41" t="n"/>
-      <c r="I43" s="41" t="n"/>
+      <c r="H43" s="14" t="n"/>
+      <c r="I43" s="14" t="n"/>
       <c r="J43" s="8" t="n"/>
-      <c r="K43" s="41" t="n"/>
-      <c r="L43" s="41" t="n"/>
+      <c r="K43" s="14" t="n"/>
+      <c r="L43" s="14" t="n"/>
       <c r="M43" s="8" t="n"/>
     </row>
     <row r="44" ht="8.1" customHeight="1" s="12">
       <c r="B44" s="45" t="inlineStr"/>
       <c r="C44" s="46" t="n"/>
-      <c r="E44" s="41" t="n"/>
-      <c r="F44" s="41" t="n"/>
+      <c r="E44" s="14" t="n"/>
+      <c r="F44" s="14" t="n"/>
       <c r="G44" s="8" t="n"/>
-      <c r="H44" s="41" t="n"/>
-      <c r="I44" s="41" t="n"/>
+      <c r="H44" s="14" t="n"/>
+      <c r="I44" s="14" t="n"/>
       <c r="J44" s="8" t="n"/>
-      <c r="K44" s="41" t="n"/>
-      <c r="L44" s="41" t="n"/>
+      <c r="K44" s="14" t="n"/>
+      <c r="L44" s="14" t="n"/>
       <c r="M44" s="8" t="n"/>
     </row>
     <row r="45" ht="8.1" customHeight="1" s="12">
-      <c r="B45" s="41" t="n"/>
-      <c r="C45" s="41" t="n"/>
+      <c r="B45" s="14" t="n"/>
+      <c r="C45" s="14" t="n"/>
       <c r="D45" s="9" t="n"/>
       <c r="E45" s="49" t="inlineStr">
         <is>
@@ -1337,16 +1337,16 @@
         </is>
       </c>
       <c r="F45" s="44" t="n"/>
-      <c r="H45" s="41" t="n"/>
-      <c r="I45" s="41" t="n"/>
+      <c r="H45" s="14" t="n"/>
+      <c r="I45" s="14" t="n"/>
       <c r="J45" s="8" t="n"/>
-      <c r="K45" s="41" t="n"/>
-      <c r="L45" s="41" t="n"/>
+      <c r="K45" s="14" t="n"/>
+      <c r="L45" s="14" t="n"/>
       <c r="M45" s="8" t="n"/>
     </row>
     <row r="46" ht="8.1" customHeight="1" s="12">
-      <c r="B46" s="41" t="n"/>
-      <c r="C46" s="41" t="n"/>
+      <c r="B46" s="14" t="n"/>
+      <c r="C46" s="14" t="n"/>
       <c r="D46" s="3" t="n"/>
       <c r="E46" s="51" t="inlineStr">
         <is>
@@ -1354,11 +1354,11 @@
         </is>
       </c>
       <c r="F46" s="46" t="n"/>
-      <c r="H46" s="41" t="n"/>
-      <c r="I46" s="41" t="n"/>
+      <c r="H46" s="14" t="n"/>
+      <c r="I46" s="14" t="n"/>
       <c r="J46" s="8" t="n"/>
-      <c r="K46" s="41" t="n"/>
-      <c r="L46" s="41" t="n"/>
+      <c r="K46" s="14" t="n"/>
+      <c r="L46" s="14" t="n"/>
       <c r="M46" s="8" t="n"/>
     </row>
     <row r="47" ht="8.1" customHeight="1" s="12">
@@ -1368,13 +1368,13 @@
         </is>
       </c>
       <c r="C47" s="44" t="n"/>
-      <c r="E47" s="41" t="n"/>
-      <c r="F47" s="41" t="n"/>
-      <c r="H47" s="41" t="n"/>
-      <c r="I47" s="41" t="n"/>
+      <c r="E47" s="14" t="n"/>
+      <c r="F47" s="14" t="n"/>
+      <c r="H47" s="14" t="n"/>
+      <c r="I47" s="14" t="n"/>
       <c r="J47" s="8" t="n"/>
-      <c r="K47" s="41" t="n"/>
-      <c r="L47" s="41" t="n"/>
+      <c r="K47" s="14" t="n"/>
+      <c r="L47" s="14" t="n"/>
       <c r="M47" s="8" t="n"/>
     </row>
     <row r="48" ht="8.1" customHeight="1" s="12">
@@ -1384,33 +1384,33 @@
         </is>
       </c>
       <c r="C48" s="46" t="n"/>
-      <c r="E48" s="41" t="n"/>
-      <c r="F48" s="41" t="n"/>
-      <c r="H48" s="41" t="n"/>
-      <c r="I48" s="41" t="n"/>
+      <c r="E48" s="14" t="n"/>
+      <c r="F48" s="14" t="n"/>
+      <c r="H48" s="14" t="n"/>
+      <c r="I48" s="14" t="n"/>
       <c r="J48" s="8" t="n"/>
-      <c r="K48" s="41" t="n"/>
-      <c r="L48" s="41" t="n"/>
+      <c r="K48" s="14" t="n"/>
+      <c r="L48" s="14" t="n"/>
       <c r="M48" s="8" t="n"/>
     </row>
     <row r="49" ht="8.1" customHeight="1" s="12">
-      <c r="B49" s="41" t="n"/>
-      <c r="C49" s="41" t="n"/>
-      <c r="E49" s="41" t="n"/>
-      <c r="F49" s="41" t="n"/>
-      <c r="H49" s="41" t="n"/>
-      <c r="I49" s="41" t="n"/>
+      <c r="B49" s="14" t="n"/>
+      <c r="C49" s="14" t="n"/>
+      <c r="E49" s="14" t="n"/>
+      <c r="F49" s="14" t="n"/>
+      <c r="H49" s="14" t="n"/>
+      <c r="I49" s="14" t="n"/>
       <c r="J49" s="9" t="n"/>
       <c r="K49" s="49" t="n"/>
       <c r="L49" s="44" t="n"/>
     </row>
     <row r="50" ht="8.1" customHeight="1" s="12">
-      <c r="B50" s="41" t="n"/>
-      <c r="C50" s="41" t="n"/>
-      <c r="E50" s="41" t="n"/>
-      <c r="F50" s="41" t="n"/>
-      <c r="H50" s="41" t="n"/>
-      <c r="I50" s="41" t="n"/>
+      <c r="B50" s="14" t="n"/>
+      <c r="C50" s="14" t="n"/>
+      <c r="E50" s="14" t="n"/>
+      <c r="F50" s="14" t="n"/>
+      <c r="H50" s="14" t="n"/>
+      <c r="I50" s="14" t="n"/>
       <c r="J50" s="8" t="n"/>
       <c r="K50" s="51" t="n"/>
       <c r="L50" s="46" t="n"/>
@@ -1422,10 +1422,10 @@
         </is>
       </c>
       <c r="C51" s="44" t="n"/>
-      <c r="E51" s="41" t="n"/>
-      <c r="F51" s="41" t="n"/>
-      <c r="H51" s="41" t="n"/>
-      <c r="I51" s="41" t="n"/>
+      <c r="E51" s="14" t="n"/>
+      <c r="F51" s="14" t="n"/>
+      <c r="H51" s="14" t="n"/>
+      <c r="I51" s="14" t="n"/>
       <c r="J51" s="8" t="n"/>
     </row>
     <row r="52" ht="8.1" customHeight="1" s="12">
@@ -1435,21 +1435,21 @@
         </is>
       </c>
       <c r="C52" s="46" t="n"/>
-      <c r="E52" s="41" t="n"/>
-      <c r="F52" s="41" t="n"/>
-      <c r="H52" s="41" t="n"/>
-      <c r="I52" s="41" t="n"/>
+      <c r="E52" s="14" t="n"/>
+      <c r="F52" s="14" t="n"/>
+      <c r="H52" s="14" t="n"/>
+      <c r="I52" s="14" t="n"/>
       <c r="J52" s="8" t="n"/>
-      <c r="M52" s="13" t="inlineStr">
+      <c r="M52" s="25" t="inlineStr">
         <is>
           <t>1st Place:</t>
         </is>
       </c>
-      <c r="N52" s="31" t="n"/>
+      <c r="N52" s="40" t="n"/>
     </row>
     <row r="53" ht="8.1" customHeight="1" s="12">
-      <c r="B53" s="41" t="n"/>
-      <c r="C53" s="41" t="n"/>
+      <c r="B53" s="14" t="n"/>
+      <c r="C53" s="14" t="n"/>
       <c r="D53" s="9" t="n"/>
       <c r="E53" s="43" t="inlineStr">
         <is>
@@ -1457,8 +1457,8 @@
         </is>
       </c>
       <c r="F53" s="44" t="n"/>
-      <c r="H53" s="41" t="n"/>
-      <c r="I53" s="41" t="n"/>
+      <c r="H53" s="14" t="n"/>
+      <c r="I53" s="14" t="n"/>
       <c r="J53" s="8" t="n"/>
       <c r="N53" s="42" t="n"/>
       <c r="O53" s="42" t="n"/>
@@ -1466,8 +1466,8 @@
       <c r="Q53" s="42" t="n"/>
     </row>
     <row r="54" ht="8.1" customHeight="1" s="12">
-      <c r="B54" s="41" t="n"/>
-      <c r="C54" s="41" t="n"/>
+      <c r="B54" s="14" t="n"/>
+      <c r="C54" s="14" t="n"/>
       <c r="D54" s="3" t="n"/>
       <c r="E54" s="45" t="inlineStr">
         <is>
@@ -1475,8 +1475,8 @@
         </is>
       </c>
       <c r="F54" s="46" t="n"/>
-      <c r="H54" s="41" t="n"/>
-      <c r="I54" s="41" t="n"/>
+      <c r="H54" s="14" t="n"/>
+      <c r="I54" s="14" t="n"/>
       <c r="J54" s="8" t="n"/>
     </row>
     <row r="55" ht="8.1" customHeight="1" s="12">
@@ -1486,27 +1486,27 @@
         </is>
       </c>
       <c r="C55" s="44" t="n"/>
-      <c r="E55" s="41" t="n"/>
-      <c r="F55" s="41" t="n"/>
+      <c r="E55" s="14" t="n"/>
+      <c r="F55" s="14" t="n"/>
       <c r="G55" s="8" t="n"/>
-      <c r="H55" s="41" t="n"/>
-      <c r="I55" s="41" t="n"/>
+      <c r="H55" s="14" t="n"/>
+      <c r="I55" s="14" t="n"/>
       <c r="J55" s="8" t="n"/>
-      <c r="M55" s="13" t="inlineStr">
+      <c r="M55" s="25" t="inlineStr">
         <is>
           <t>2nd Place:</t>
         </is>
       </c>
-      <c r="N55" s="31" t="n"/>
+      <c r="N55" s="40" t="n"/>
     </row>
     <row r="56" ht="8.1" customHeight="1" s="12">
       <c r="B56" s="51" t="inlineStr"/>
       <c r="C56" s="46" t="n"/>
-      <c r="E56" s="41" t="n"/>
-      <c r="F56" s="41" t="n"/>
+      <c r="E56" s="14" t="n"/>
+      <c r="F56" s="14" t="n"/>
       <c r="G56" s="8" t="n"/>
-      <c r="H56" s="41" t="n"/>
-      <c r="I56" s="41" t="n"/>
+      <c r="H56" s="14" t="n"/>
+      <c r="I56" s="14" t="n"/>
       <c r="J56" s="8" t="n"/>
       <c r="N56" s="42" t="n"/>
       <c r="O56" s="42" t="n"/>
@@ -1514,28 +1514,28 @@
       <c r="Q56" s="42" t="n"/>
     </row>
     <row r="57" ht="8.1" customHeight="1" s="12">
-      <c r="B57" s="41" t="n"/>
-      <c r="C57" s="41" t="n"/>
-      <c r="E57" s="41" t="n"/>
-      <c r="F57" s="41" t="n"/>
+      <c r="B57" s="14" t="n"/>
+      <c r="C57" s="14" t="n"/>
+      <c r="E57" s="14" t="n"/>
+      <c r="F57" s="14" t="n"/>
       <c r="G57" s="9" t="n"/>
       <c r="H57" s="49" t="n"/>
       <c r="I57" s="44" t="n"/>
     </row>
     <row r="58" ht="8.1" customHeight="1" s="12">
-      <c r="B58" s="41" t="n"/>
-      <c r="C58" s="41" t="n"/>
-      <c r="E58" s="41" t="n"/>
-      <c r="F58" s="41" t="n"/>
+      <c r="B58" s="14" t="n"/>
+      <c r="C58" s="14" t="n"/>
+      <c r="E58" s="14" t="n"/>
+      <c r="F58" s="14" t="n"/>
       <c r="G58" s="8" t="n"/>
       <c r="H58" s="51" t="n"/>
       <c r="I58" s="46" t="n"/>
-      <c r="M58" s="13" t="inlineStr">
+      <c r="M58" s="25" t="inlineStr">
         <is>
           <t>3rd Place:</t>
         </is>
       </c>
-      <c r="N58" s="31" t="n"/>
+      <c r="N58" s="40" t="n"/>
     </row>
     <row r="59" ht="8.1" customHeight="1" s="12">
       <c r="B59" s="43" t="inlineStr">
@@ -1544,8 +1544,8 @@
         </is>
       </c>
       <c r="C59" s="44" t="n"/>
-      <c r="E59" s="41" t="n"/>
-      <c r="F59" s="41" t="n"/>
+      <c r="E59" s="14" t="n"/>
+      <c r="F59" s="14" t="n"/>
       <c r="G59" s="8" t="n"/>
       <c r="N59" s="42" t="n"/>
       <c r="O59" s="42" t="n"/>
@@ -1555,13 +1555,13 @@
     <row r="60" ht="8.1" customHeight="1" s="12">
       <c r="B60" s="45" t="inlineStr"/>
       <c r="C60" s="46" t="n"/>
-      <c r="E60" s="41" t="n"/>
-      <c r="F60" s="41" t="n"/>
+      <c r="E60" s="14" t="n"/>
+      <c r="F60" s="14" t="n"/>
       <c r="G60" s="8" t="n"/>
     </row>
     <row r="61" ht="8.1" customHeight="1" s="12">
-      <c r="B61" s="41" t="n"/>
-      <c r="C61" s="41" t="n"/>
+      <c r="B61" s="14" t="n"/>
+      <c r="C61" s="14" t="n"/>
       <c r="D61" s="9" t="n"/>
       <c r="E61" s="49" t="inlineStr">
         <is>
@@ -1569,16 +1569,16 @@
         </is>
       </c>
       <c r="F61" s="44" t="n"/>
-      <c r="M61" s="13" t="inlineStr">
+      <c r="M61" s="25" t="inlineStr">
         <is>
           <t>3rd Place:</t>
         </is>
       </c>
-      <c r="N61" s="31" t="n"/>
+      <c r="N61" s="40" t="n"/>
     </row>
     <row r="62" ht="8.1" customHeight="1" s="12">
-      <c r="B62" s="41" t="n"/>
-      <c r="C62" s="41" t="n"/>
+      <c r="B62" s="14" t="n"/>
+      <c r="C62" s="14" t="n"/>
       <c r="D62" s="3" t="n"/>
       <c r="E62" s="51" t="inlineStr">
         <is>
@@ -1616,38 +1616,34 @@
     <row r="71" ht="8.1" customHeight="1" s="12"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="M55:M56"/>
+    <mergeCell ref="M58:M59"/>
+    <mergeCell ref="M61:M62"/>
+    <mergeCell ref="K6:Q9"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N31:O32"/>
+    <mergeCell ref="N52:Q53"/>
+    <mergeCell ref="N55:Q56"/>
+    <mergeCell ref="N58:Q59"/>
+    <mergeCell ref="N61:Q62"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="K1:L2"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="E5:F5"/>
@@ -1664,34 +1660,38 @@
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="E1:F2"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="K1:L2"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="M55:M56"/>
-    <mergeCell ref="M58:M59"/>
-    <mergeCell ref="M61:M62"/>
-    <mergeCell ref="K6:Q9"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="N31:O32"/>
-    <mergeCell ref="N52:Q53"/>
-    <mergeCell ref="N55:Q56"/>
-    <mergeCell ref="N58:Q59"/>
-    <mergeCell ref="N61:Q62"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>